<commit_message>
Gure nominak eginda baina ez daude guztiz bukatuta, mirenen erantzunaz zain
</commit_message>
<xml_diff>
--- a/Nominak/Nomina1.xlsx
+++ b/Nominak/Nomina1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\3Erronka\Nominak\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7135CFE0-2C27-415D-86A0-9AEDA2A0B426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7651323D-9892-4759-88D0-7DCCCD09BD82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{26F0538E-6B62-47F3-88A6-EBF291EB1297}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="99">
   <si>
     <t>Enpresa:</t>
   </si>
@@ -338,19 +338,25 @@
     <t>100</t>
   </si>
   <si>
-    <t>Iker Lopez</t>
-  </si>
-  <si>
-    <t>123456789A</t>
-  </si>
-  <si>
-    <t>8676329</t>
-  </si>
-  <si>
     <t>martxoa</t>
   </si>
   <si>
     <t>apirila</t>
+  </si>
+  <si>
+    <t>Oier Talavera</t>
+  </si>
+  <si>
+    <t>34363438N</t>
+  </si>
+  <si>
+    <t>9482856</t>
+  </si>
+  <si>
+    <t>Pizgarriak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allurralde </t>
   </si>
 </sst>
 </file>
@@ -720,6 +726,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -771,7 +778,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1109,10 +1115,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:W74"/>
+  <dimension ref="A1:X74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W41" sqref="W41"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5:T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1140,158 +1146,156 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="67" t="s">
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="68" t="s">
         <v>88</v>
       </c>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="67"/>
-      <c r="L1" s="67"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
       <c r="M1" s="3"/>
       <c r="O1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="P1" s="79" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q1" s="79"/>
-      <c r="R1" s="79"/>
-      <c r="S1" s="79"/>
-      <c r="T1" s="79"/>
+      <c r="P1" s="80" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q1" s="80"/>
+      <c r="R1" s="80"/>
+      <c r="S1" s="80"/>
+      <c r="T1" s="80"/>
       <c r="U1" s="3"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A2" s="68" t="s">
+      <c r="A2" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="67" t="s">
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="68" t="s">
         <v>89</v>
       </c>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
-      <c r="L2" s="67"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="68"/>
       <c r="M2" s="5"/>
       <c r="O2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="P2" s="69" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q2" s="69"/>
-      <c r="R2" s="69"/>
-      <c r="S2" s="69"/>
-      <c r="T2" s="69"/>
+      <c r="P2" s="70" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q2" s="70"/>
+      <c r="R2" s="70"/>
+      <c r="S2" s="70"/>
+      <c r="T2" s="70"/>
       <c r="U2" s="5"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A3" s="68" t="s">
+      <c r="A3" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="67" t="s">
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="68" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="67"/>
-      <c r="L3" s="67"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
+      <c r="L3" s="68"/>
       <c r="M3" s="5"/>
       <c r="O3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="P3" s="76" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q3" s="69"/>
-      <c r="R3" s="69"/>
-      <c r="S3" s="69"/>
-      <c r="T3" s="69"/>
+      <c r="P3" s="77" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q3" s="70"/>
+      <c r="R3" s="70"/>
+      <c r="S3" s="70"/>
+      <c r="T3" s="70"/>
       <c r="U3" s="5"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A4" s="68" t="s">
+      <c r="A4" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
-      <c r="J4" s="67"/>
-      <c r="K4" s="67"/>
-      <c r="L4" s="67"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="68"/>
+      <c r="I4" s="68"/>
+      <c r="J4" s="68"/>
+      <c r="K4" s="68"/>
+      <c r="L4" s="68"/>
       <c r="M4" s="5"/>
       <c r="O4" s="4" t="s">
         <v>28</v>
       </c>
       <c r="P4" s="6"/>
-      <c r="Q4" s="77" t="s">
+      <c r="Q4" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="R4" s="77"/>
-      <c r="S4" s="77"/>
-      <c r="T4" s="77"/>
+      <c r="R4" s="78"/>
+      <c r="S4" s="78"/>
+      <c r="T4" s="78"/>
       <c r="U4" s="5"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A5" s="68" t="s">
+      <c r="A5" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="69" t="s">
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="70" t="s">
         <v>91</v>
       </c>
-      <c r="F5" s="69"/>
-      <c r="G5" s="69"/>
-      <c r="H5" s="69"/>
-      <c r="I5" s="69"/>
-      <c r="J5" s="69"/>
-      <c r="K5" s="69"/>
-      <c r="L5" s="69"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="70"/>
+      <c r="I5" s="70"/>
+      <c r="J5" s="70"/>
+      <c r="K5" s="70"/>
+      <c r="L5" s="70"/>
       <c r="M5" s="5"/>
       <c r="O5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="P5" s="53">
-        <v>5</v>
-      </c>
-      <c r="Q5" s="70"/>
-      <c r="R5" s="70"/>
-      <c r="S5" s="70"/>
-      <c r="T5" s="70"/>
+      <c r="P5" s="54"/>
+      <c r="Q5" s="71"/>
+      <c r="R5" s="71"/>
+      <c r="S5" s="71"/>
+      <c r="T5" s="71"/>
       <c r="U5" s="5"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A6" s="71"/>
-      <c r="B6" s="72"/>
-      <c r="C6" s="72"/>
-      <c r="D6" s="72"/>
+      <c r="A6" s="72"/>
+      <c r="B6" s="73"/>
+      <c r="C6" s="73"/>
+      <c r="D6" s="73"/>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
@@ -1310,13 +1314,13 @@
       <c r="U6" s="12"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A8" s="73" t="s">
+      <c r="A8" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="74"/>
-      <c r="C8" s="74"/>
-      <c r="D8" s="74"/>
-      <c r="E8" s="74"/>
+      <c r="B8" s="75"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="75"/>
+      <c r="E8" s="75"/>
       <c r="F8" s="7">
         <v>2025</v>
       </c>
@@ -1324,7 +1328,7 @@
         <v>31</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="I8" s="43" t="s">
         <v>32</v>
@@ -1337,7 +1341,7 @@
         <v>33</v>
       </c>
       <c r="M8" s="42" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="N8" s="2" t="s">
         <v>32</v>
@@ -1424,26 +1428,26 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
-      <c r="C13" s="45" t="s">
+      <c r="C13" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="45"/>
-      <c r="I13" s="45"/>
-      <c r="J13" s="45"/>
-      <c r="K13" s="45"/>
-      <c r="L13" s="45"/>
-      <c r="M13" s="45"/>
-      <c r="N13" s="45"/>
-      <c r="O13" s="45"/>
-      <c r="P13" s="57">
+      <c r="D13" s="46"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="46"/>
+      <c r="I13" s="46"/>
+      <c r="J13" s="46"/>
+      <c r="K13" s="46"/>
+      <c r="L13" s="46"/>
+      <c r="M13" s="46"/>
+      <c r="N13" s="46"/>
+      <c r="O13" s="46"/>
+      <c r="P13" s="58">
         <v>1856.11</v>
       </c>
-      <c r="Q13" s="57"/>
-      <c r="R13" s="57"/>
+      <c r="Q13" s="58"/>
+      <c r="R13" s="58"/>
       <c r="U13" s="5"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
@@ -1451,184 +1455,188 @@
       <c r="C14" t="s">
         <v>39</v>
       </c>
-      <c r="P14" s="75"/>
-      <c r="Q14" s="75"/>
-      <c r="R14" s="75"/>
+      <c r="P14" s="76"/>
+      <c r="Q14" s="76"/>
+      <c r="R14" s="76"/>
       <c r="U14" s="5"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="52"/>
-      <c r="H15" s="52"/>
-      <c r="I15" s="52"/>
-      <c r="J15" s="52"/>
-      <c r="K15" s="52"/>
-      <c r="L15" s="52"/>
-      <c r="M15" s="52"/>
-      <c r="N15" s="52"/>
+      <c r="D15" s="53" t="s">
+        <v>97</v>
+      </c>
+      <c r="E15" s="53"/>
+      <c r="F15" s="53"/>
+      <c r="G15" s="53"/>
+      <c r="H15" s="53"/>
+      <c r="I15" s="53"/>
+      <c r="J15" s="53"/>
+      <c r="K15" s="53"/>
+      <c r="L15" s="53"/>
+      <c r="M15" s="53"/>
+      <c r="N15" s="53"/>
       <c r="O15" t="s">
         <v>8</v>
       </c>
-      <c r="P15" s="57">
+      <c r="P15" s="58">
         <v>230</v>
       </c>
-      <c r="Q15" s="57"/>
-      <c r="R15" s="57"/>
+      <c r="Q15" s="58"/>
+      <c r="R15" s="58"/>
       <c r="U15" s="5"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="52"/>
-      <c r="I16" s="52"/>
-      <c r="J16" s="52"/>
-      <c r="K16" s="52"/>
-      <c r="L16" s="52"/>
-      <c r="M16" s="52"/>
-      <c r="N16" s="52"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="53"/>
+      <c r="G16" s="53"/>
+      <c r="H16" s="53"/>
+      <c r="I16" s="53"/>
+      <c r="J16" s="53"/>
+      <c r="K16" s="53"/>
+      <c r="L16" s="53"/>
+      <c r="M16" s="53"/>
+      <c r="N16" s="53"/>
       <c r="O16" t="s">
         <v>8</v>
       </c>
-      <c r="P16" s="57"/>
-      <c r="Q16" s="57"/>
-      <c r="R16" s="57"/>
+      <c r="P16" s="58"/>
+      <c r="Q16" s="58"/>
+      <c r="R16" s="58"/>
       <c r="U16" s="5"/>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
-      <c r="D17" s="67"/>
-      <c r="E17" s="67"/>
-      <c r="F17" s="67"/>
-      <c r="G17" s="67"/>
-      <c r="H17" s="67"/>
-      <c r="I17" s="67"/>
-      <c r="J17" s="67"/>
-      <c r="K17" s="67"/>
-      <c r="L17" s="67"/>
-      <c r="M17" s="67"/>
-      <c r="N17" s="67"/>
+      <c r="D17" s="68"/>
+      <c r="E17" s="68"/>
+      <c r="F17" s="68"/>
+      <c r="G17" s="68"/>
+      <c r="H17" s="68"/>
+      <c r="I17" s="68"/>
+      <c r="J17" s="68"/>
+      <c r="K17" s="68"/>
+      <c r="L17" s="68"/>
+      <c r="M17" s="68"/>
+      <c r="N17" s="68"/>
       <c r="O17" t="s">
         <v>8</v>
       </c>
-      <c r="P17" s="57"/>
-      <c r="Q17" s="57"/>
-      <c r="R17" s="57"/>
+      <c r="P17" s="58"/>
+      <c r="Q17" s="58"/>
+      <c r="R17" s="58"/>
       <c r="U17" s="5"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
-      <c r="C18" s="45" t="s">
+      <c r="C18" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="45"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="45"/>
-      <c r="I18" s="45"/>
-      <c r="J18" s="45"/>
-      <c r="K18" s="45"/>
-      <c r="L18" s="45"/>
-      <c r="M18" s="45"/>
-      <c r="N18" s="45"/>
-      <c r="O18" s="45"/>
-      <c r="P18" s="57"/>
-      <c r="Q18" s="57"/>
-      <c r="R18" s="57"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="46"/>
+      <c r="K18" s="46"/>
+      <c r="L18" s="46"/>
+      <c r="M18" s="46"/>
+      <c r="N18" s="46"/>
+      <c r="O18" s="46"/>
+      <c r="P18" s="58">
+        <v>160</v>
+      </c>
+      <c r="Q18" s="58"/>
+      <c r="R18" s="58"/>
       <c r="U18" s="5"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
-      <c r="C19" s="45" t="s">
+      <c r="C19" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="45"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="45"/>
-      <c r="G19" s="45"/>
-      <c r="H19" s="45"/>
-      <c r="I19" s="45"/>
-      <c r="J19" s="45"/>
-      <c r="K19" s="45"/>
-      <c r="L19" s="45"/>
-      <c r="M19" s="45"/>
-      <c r="N19" s="45"/>
-      <c r="O19" s="45"/>
-      <c r="P19" s="57"/>
-      <c r="Q19" s="57"/>
-      <c r="R19" s="57"/>
+      <c r="D19" s="46"/>
+      <c r="E19" s="46"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="46"/>
+      <c r="H19" s="46"/>
+      <c r="I19" s="46"/>
+      <c r="J19" s="46"/>
+      <c r="K19" s="46"/>
+      <c r="L19" s="46"/>
+      <c r="M19" s="46"/>
+      <c r="N19" s="46"/>
+      <c r="O19" s="46"/>
+      <c r="P19" s="58"/>
+      <c r="Q19" s="58"/>
+      <c r="R19" s="58"/>
       <c r="U19" s="5"/>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
-      <c r="C20" s="66" t="s">
+      <c r="C20" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="45"/>
-      <c r="E20" s="45"/>
-      <c r="F20" s="45"/>
-      <c r="G20" s="45"/>
-      <c r="H20" s="45"/>
-      <c r="I20" s="45"/>
-      <c r="J20" s="45"/>
-      <c r="K20" s="45"/>
-      <c r="L20" s="45"/>
-      <c r="M20" s="45"/>
-      <c r="N20" s="45"/>
-      <c r="O20" s="45"/>
-      <c r="P20" s="57"/>
-      <c r="Q20" s="57"/>
-      <c r="R20" s="57"/>
+      <c r="D20" s="46"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="46"/>
+      <c r="H20" s="46"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="46"/>
+      <c r="K20" s="46"/>
+      <c r="L20" s="46"/>
+      <c r="M20" s="46"/>
+      <c r="N20" s="46"/>
+      <c r="O20" s="46"/>
+      <c r="P20" s="58"/>
+      <c r="Q20" s="58"/>
+      <c r="R20" s="58"/>
       <c r="U20" s="5"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
-      <c r="C21" s="45" t="s">
+      <c r="C21" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="45"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="45"/>
-      <c r="G21" s="45"/>
-      <c r="H21" s="45"/>
-      <c r="I21" s="45"/>
-      <c r="J21" s="45"/>
-      <c r="K21" s="45"/>
-      <c r="L21" s="45"/>
-      <c r="M21" s="45"/>
-      <c r="N21" s="45"/>
-      <c r="O21" s="45"/>
-      <c r="P21" s="57"/>
-      <c r="Q21" s="57"/>
-      <c r="R21" s="57"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="46"/>
+      <c r="K21" s="46"/>
+      <c r="L21" s="46"/>
+      <c r="M21" s="46"/>
+      <c r="N21" s="46"/>
+      <c r="O21" s="46"/>
+      <c r="P21" s="58"/>
+      <c r="Q21" s="58"/>
+      <c r="R21" s="58"/>
       <c r="U21" s="5"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
-      <c r="C22" s="45" t="s">
+      <c r="C22" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="45"/>
-      <c r="E22" s="45"/>
-      <c r="F22" s="45"/>
-      <c r="G22" s="45"/>
-      <c r="H22" s="45"/>
-      <c r="I22" s="45"/>
-      <c r="J22" s="45"/>
-      <c r="K22" s="45"/>
-      <c r="L22" s="45"/>
-      <c r="M22" s="45"/>
-      <c r="N22" s="45"/>
-      <c r="O22" s="45"/>
-      <c r="P22" s="57"/>
-      <c r="Q22" s="57"/>
-      <c r="R22" s="57"/>
+      <c r="D22" s="46"/>
+      <c r="E22" s="46"/>
+      <c r="F22" s="46"/>
+      <c r="G22" s="46"/>
+      <c r="H22" s="46"/>
+      <c r="I22" s="46"/>
+      <c r="J22" s="46"/>
+      <c r="K22" s="46"/>
+      <c r="L22" s="46"/>
+      <c r="M22" s="46"/>
+      <c r="N22" s="46"/>
+      <c r="O22" s="46"/>
+      <c r="P22" s="58"/>
+      <c r="Q22" s="58"/>
+      <c r="R22" s="58"/>
       <c r="U22" s="5"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.3">
@@ -1654,65 +1662,65 @@
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
-      <c r="D26" s="52"/>
-      <c r="E26" s="52"/>
-      <c r="F26" s="52"/>
-      <c r="G26" s="52"/>
-      <c r="H26" s="52"/>
-      <c r="I26" s="52"/>
-      <c r="J26" s="52"/>
-      <c r="K26" s="52"/>
-      <c r="L26" s="52"/>
-      <c r="M26" s="52"/>
-      <c r="N26" s="52"/>
+      <c r="D26" s="53"/>
+      <c r="E26" s="53"/>
+      <c r="F26" s="53"/>
+      <c r="G26" s="53"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="53"/>
+      <c r="J26" s="53"/>
+      <c r="K26" s="53"/>
+      <c r="L26" s="53"/>
+      <c r="M26" s="53"/>
+      <c r="N26" s="53"/>
       <c r="O26" t="s">
         <v>8</v>
       </c>
-      <c r="P26" s="57"/>
-      <c r="Q26" s="57"/>
-      <c r="R26" s="57"/>
+      <c r="P26" s="58"/>
+      <c r="Q26" s="58"/>
+      <c r="R26" s="58"/>
       <c r="U26" s="5"/>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
-      <c r="D27" s="52"/>
-      <c r="E27" s="52"/>
-      <c r="F27" s="52"/>
-      <c r="G27" s="52"/>
-      <c r="H27" s="52"/>
-      <c r="I27" s="52"/>
-      <c r="J27" s="52"/>
-      <c r="K27" s="52"/>
-      <c r="L27" s="52"/>
-      <c r="M27" s="52"/>
-      <c r="N27" s="52"/>
+      <c r="D27" s="53"/>
+      <c r="E27" s="53"/>
+      <c r="F27" s="53"/>
+      <c r="G27" s="53"/>
+      <c r="H27" s="53"/>
+      <c r="I27" s="53"/>
+      <c r="J27" s="53"/>
+      <c r="K27" s="53"/>
+      <c r="L27" s="53"/>
+      <c r="M27" s="53"/>
+      <c r="N27" s="53"/>
       <c r="O27" t="s">
         <v>8</v>
       </c>
-      <c r="P27" s="57"/>
-      <c r="Q27" s="57"/>
-      <c r="R27" s="57"/>
+      <c r="P27" s="58"/>
+      <c r="Q27" s="58"/>
+      <c r="R27" s="58"/>
       <c r="U27" s="5"/>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
-      <c r="D28" s="52"/>
-      <c r="E28" s="52"/>
-      <c r="F28" s="52"/>
-      <c r="G28" s="52"/>
-      <c r="H28" s="52"/>
-      <c r="I28" s="52"/>
-      <c r="J28" s="52"/>
-      <c r="K28" s="52"/>
-      <c r="L28" s="52"/>
-      <c r="M28" s="52"/>
-      <c r="N28" s="52"/>
+      <c r="D28" s="53"/>
+      <c r="E28" s="53"/>
+      <c r="F28" s="53"/>
+      <c r="G28" s="53"/>
+      <c r="H28" s="53"/>
+      <c r="I28" s="53"/>
+      <c r="J28" s="53"/>
+      <c r="K28" s="53"/>
+      <c r="L28" s="53"/>
+      <c r="M28" s="53"/>
+      <c r="N28" s="53"/>
       <c r="O28" t="s">
         <v>8</v>
       </c>
-      <c r="P28" s="57"/>
-      <c r="Q28" s="57"/>
-      <c r="R28" s="57"/>
+      <c r="P28" s="58"/>
+      <c r="Q28" s="58"/>
+      <c r="R28" s="58"/>
       <c r="U28" s="5"/>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.3">
@@ -1724,23 +1732,23 @@
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
-      <c r="D30" s="52"/>
-      <c r="E30" s="52"/>
-      <c r="F30" s="52"/>
-      <c r="G30" s="52"/>
-      <c r="H30" s="52"/>
-      <c r="I30" s="52"/>
-      <c r="J30" s="52"/>
-      <c r="K30" s="52"/>
-      <c r="L30" s="52"/>
-      <c r="M30" s="52"/>
-      <c r="N30" s="52"/>
+      <c r="D30" s="53"/>
+      <c r="E30" s="53"/>
+      <c r="F30" s="53"/>
+      <c r="G30" s="53"/>
+      <c r="H30" s="53"/>
+      <c r="I30" s="53"/>
+      <c r="J30" s="53"/>
+      <c r="K30" s="53"/>
+      <c r="L30" s="53"/>
+      <c r="M30" s="53"/>
+      <c r="N30" s="53"/>
       <c r="O30" t="s">
         <v>8</v>
       </c>
-      <c r="P30" s="57"/>
-      <c r="Q30" s="57"/>
-      <c r="R30" s="57"/>
+      <c r="P30" s="58"/>
+      <c r="Q30" s="58"/>
+      <c r="R30" s="58"/>
       <c r="U30" s="5"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.3">
@@ -1755,23 +1763,23 @@
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
-      <c r="D32" s="52"/>
-      <c r="E32" s="52"/>
-      <c r="F32" s="52"/>
-      <c r="G32" s="52"/>
-      <c r="H32" s="52"/>
-      <c r="I32" s="52"/>
-      <c r="J32" s="52"/>
-      <c r="K32" s="52"/>
-      <c r="L32" s="52"/>
-      <c r="M32" s="52"/>
-      <c r="N32" s="52"/>
+      <c r="D32" s="53"/>
+      <c r="E32" s="53"/>
+      <c r="F32" s="53"/>
+      <c r="G32" s="53"/>
+      <c r="H32" s="53"/>
+      <c r="I32" s="53"/>
+      <c r="J32" s="53"/>
+      <c r="K32" s="53"/>
+      <c r="L32" s="53"/>
+      <c r="M32" s="53"/>
+      <c r="N32" s="53"/>
       <c r="O32" t="s">
         <v>8</v>
       </c>
-      <c r="P32" s="57"/>
-      <c r="Q32" s="57"/>
-      <c r="R32" s="57"/>
+      <c r="P32" s="58"/>
+      <c r="Q32" s="58"/>
+      <c r="R32" s="58"/>
       <c r="U32" s="5"/>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.3">
@@ -1786,23 +1794,23 @@
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
-      <c r="D34" s="52"/>
-      <c r="E34" s="52"/>
-      <c r="F34" s="52"/>
-      <c r="G34" s="52"/>
-      <c r="H34" s="52"/>
-      <c r="I34" s="52"/>
-      <c r="J34" s="52"/>
-      <c r="K34" s="52"/>
-      <c r="L34" s="52"/>
-      <c r="M34" s="52"/>
-      <c r="N34" s="52"/>
+      <c r="D34" s="53"/>
+      <c r="E34" s="53"/>
+      <c r="F34" s="53"/>
+      <c r="G34" s="53"/>
+      <c r="H34" s="53"/>
+      <c r="I34" s="53"/>
+      <c r="J34" s="53"/>
+      <c r="K34" s="53"/>
+      <c r="L34" s="53"/>
+      <c r="M34" s="53"/>
+      <c r="N34" s="53"/>
       <c r="O34" t="s">
         <v>8</v>
       </c>
-      <c r="P34" s="57"/>
-      <c r="Q34" s="57"/>
-      <c r="R34" s="57"/>
+      <c r="P34" s="58"/>
+      <c r="Q34" s="58"/>
+      <c r="R34" s="58"/>
       <c r="U34" s="5"/>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.3">
@@ -1811,23 +1819,23 @@
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
-      <c r="I36" s="48" t="s">
+      <c r="I36" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="J36" s="48"/>
-      <c r="K36" s="48"/>
-      <c r="L36" s="48"/>
-      <c r="M36" s="48"/>
-      <c r="N36" s="48"/>
-      <c r="O36" s="48"/>
-      <c r="P36" s="48"/>
-      <c r="Q36" s="48"/>
-      <c r="R36" s="48"/>
-      <c r="S36" s="58">
+      <c r="J36" s="49"/>
+      <c r="K36" s="49"/>
+      <c r="L36" s="49"/>
+      <c r="M36" s="49"/>
+      <c r="N36" s="49"/>
+      <c r="O36" s="49"/>
+      <c r="P36" s="49"/>
+      <c r="Q36" s="49"/>
+      <c r="R36" s="49"/>
+      <c r="S36" s="59">
         <f>P13+P15+P16+P17+P18+P19+P20+P21+P22+P26+P27+P28+P30+P32+P34</f>
-        <v>2086.1099999999997</v>
-      </c>
-      <c r="T36" s="58"/>
+        <v>2246.1099999999997</v>
+      </c>
+      <c r="T36" s="59"/>
       <c r="U36" s="5"/>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.3">
@@ -1866,14 +1874,14 @@
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A40" s="4"/>
-      <c r="D40" s="55" t="s">
+      <c r="D40" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="E40" s="56"/>
-      <c r="F40" s="56"/>
-      <c r="G40" s="56"/>
-      <c r="H40" s="56"/>
-      <c r="I40" s="56"/>
+      <c r="E40" s="57"/>
+      <c r="F40" s="57"/>
+      <c r="G40" s="57"/>
+      <c r="H40" s="57"/>
+      <c r="I40" s="57"/>
       <c r="J40" s="20"/>
       <c r="K40" s="25">
         <v>4.7</v>
@@ -1881,23 +1889,23 @@
       <c r="L40" t="s">
         <v>12</v>
       </c>
-      <c r="N40" s="57">
+      <c r="N40" s="58">
         <f>+Q66*0.047</f>
-        <v>98.04716999999998</v>
-      </c>
-      <c r="O40" s="57"/>
+        <v>105.09716999999999</v>
+      </c>
+      <c r="O40" s="58"/>
       <c r="V40" s="4"/>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A41" s="4"/>
-      <c r="D41" s="55" t="s">
+      <c r="D41" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="E41" s="56"/>
-      <c r="F41" s="56"/>
-      <c r="G41" s="56"/>
-      <c r="H41" s="56"/>
-      <c r="I41" s="56"/>
+      <c r="E41" s="57"/>
+      <c r="F41" s="57"/>
+      <c r="G41" s="57"/>
+      <c r="H41" s="57"/>
+      <c r="I41" s="57"/>
       <c r="J41" s="20"/>
       <c r="K41" s="25">
         <v>1.55</v>
@@ -1905,24 +1913,24 @@
       <c r="L41" t="s">
         <v>12</v>
       </c>
-      <c r="N41" s="57">
+      <c r="N41" s="58">
         <f>Q69*0.0155</f>
-        <v>32.334704999999992</v>
-      </c>
-      <c r="O41" s="57"/>
+        <v>37.139704999999992</v>
+      </c>
+      <c r="O41" s="58"/>
       <c r="U41" s="5"/>
-      <c r="W41" s="80"/>
+      <c r="W41" s="45"/>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A42" s="4"/>
-      <c r="D42" s="55" t="s">
+      <c r="D42" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="E42" s="56"/>
-      <c r="F42" s="56"/>
-      <c r="G42" s="56"/>
-      <c r="H42" s="56"/>
-      <c r="I42" s="56"/>
+      <c r="E42" s="57"/>
+      <c r="F42" s="57"/>
+      <c r="G42" s="57"/>
+      <c r="H42" s="57"/>
+      <c r="I42" s="57"/>
       <c r="J42" s="20"/>
       <c r="K42" s="25">
         <v>0.1</v>
@@ -1930,23 +1938,23 @@
       <c r="L42" t="s">
         <v>12</v>
       </c>
-      <c r="N42" s="57">
+      <c r="N42" s="58">
         <f>Q69*0.001</f>
-        <v>2.0861099999999997</v>
-      </c>
-      <c r="O42" s="57"/>
+        <v>2.3961099999999997</v>
+      </c>
+      <c r="O42" s="58"/>
       <c r="U42" s="5"/>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A43" s="4"/>
-      <c r="D43" s="55" t="s">
+      <c r="D43" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="E43" s="56"/>
-      <c r="F43" s="56"/>
-      <c r="G43" s="56"/>
-      <c r="H43" s="56"/>
-      <c r="I43" s="56"/>
+      <c r="E43" s="57"/>
+      <c r="F43" s="57"/>
+      <c r="G43" s="57"/>
+      <c r="H43" s="57"/>
+      <c r="I43" s="57"/>
       <c r="J43" s="20"/>
       <c r="K43" s="25">
         <v>2</v>
@@ -1954,23 +1962,23 @@
       <c r="L43" t="s">
         <v>12</v>
       </c>
-      <c r="N43" s="57">
+      <c r="N43" s="58">
         <f>O71*0.02</f>
-        <v>0</v>
-      </c>
-      <c r="O43" s="57"/>
+        <v>3.2</v>
+      </c>
+      <c r="O43" s="58"/>
       <c r="U43" s="5"/>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A44" s="4"/>
-      <c r="D44" s="55" t="s">
+      <c r="D44" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="E44" s="56"/>
-      <c r="F44" s="56"/>
-      <c r="G44" s="56"/>
-      <c r="H44" s="56"/>
-      <c r="I44" s="56"/>
+      <c r="E44" s="57"/>
+      <c r="F44" s="57"/>
+      <c r="G44" s="57"/>
+      <c r="H44" s="57"/>
+      <c r="I44" s="57"/>
       <c r="J44" s="20"/>
       <c r="K44" s="25">
         <v>4.7</v>
@@ -1978,35 +1986,35 @@
       <c r="L44" t="s">
         <v>12</v>
       </c>
-      <c r="N44" s="57">
+      <c r="N44" s="58">
         <f>O72*0.047</f>
         <v>0</v>
       </c>
-      <c r="O44" s="57"/>
+      <c r="O44" s="58"/>
       <c r="U44" s="5"/>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A45" s="4"/>
       <c r="D45" s="26"/>
-      <c r="E45" s="55" t="s">
+      <c r="E45" s="56" t="s">
         <v>56</v>
       </c>
-      <c r="F45" s="56"/>
-      <c r="G45" s="56"/>
-      <c r="H45" s="56"/>
-      <c r="I45" s="56"/>
-      <c r="J45" s="56"/>
-      <c r="K45" s="56"/>
-      <c r="L45" s="56"/>
-      <c r="M45" s="56"/>
-      <c r="N45" s="56"/>
-      <c r="O45" s="56"/>
-      <c r="P45" s="57">
+      <c r="F45" s="57"/>
+      <c r="G45" s="57"/>
+      <c r="H45" s="57"/>
+      <c r="I45" s="57"/>
+      <c r="J45" s="57"/>
+      <c r="K45" s="57"/>
+      <c r="L45" s="57"/>
+      <c r="M45" s="57"/>
+      <c r="N45" s="57"/>
+      <c r="O45" s="57"/>
+      <c r="P45" s="58">
         <f>N40+N41+N42+N43+N44</f>
-        <v>132.46798499999997</v>
-      </c>
-      <c r="Q45" s="57"/>
-      <c r="R45" s="57"/>
+        <v>147.83298499999998</v>
+      </c>
+      <c r="Q45" s="58"/>
+      <c r="R45" s="58"/>
       <c r="U45" s="5"/>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.3">
@@ -2014,14 +2022,14 @@
       <c r="C46" t="s">
         <v>13</v>
       </c>
-      <c r="D46" s="64" t="s">
+      <c r="D46" s="65" t="s">
         <v>57</v>
       </c>
-      <c r="E46" s="65"/>
-      <c r="F46" s="65"/>
-      <c r="G46" s="65"/>
-      <c r="H46" s="65"/>
-      <c r="I46" s="65"/>
+      <c r="E46" s="66"/>
+      <c r="F46" s="66"/>
+      <c r="G46" s="66"/>
+      <c r="H46" s="66"/>
+      <c r="I46" s="66"/>
       <c r="J46" s="27"/>
       <c r="K46" s="25">
         <v>8</v>
@@ -2029,17 +2037,17 @@
       <c r="L46" t="s">
         <v>12</v>
       </c>
-      <c r="M46" s="45" t="s">
+      <c r="M46" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="N46" s="45"/>
-      <c r="O46" s="45"/>
-      <c r="P46" s="57">
+      <c r="N46" s="46"/>
+      <c r="O46" s="46"/>
+      <c r="P46" s="58">
         <f>O73*K46/100</f>
-        <v>166.88879999999997</v>
-      </c>
-      <c r="Q46" s="57"/>
-      <c r="R46" s="57"/>
+        <v>179.68879999999999</v>
+      </c>
+      <c r="Q46" s="58"/>
+      <c r="R46" s="58"/>
       <c r="U46" s="5"/>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.3">
@@ -2047,23 +2055,23 @@
       <c r="C47" t="s">
         <v>15</v>
       </c>
-      <c r="D47" s="55" t="s">
+      <c r="D47" s="56" t="s">
         <v>58</v>
       </c>
-      <c r="E47" s="56"/>
-      <c r="F47" s="56"/>
-      <c r="G47" s="56"/>
-      <c r="H47" s="56"/>
-      <c r="I47" s="56"/>
-      <c r="J47" s="56"/>
-      <c r="K47" s="56"/>
-      <c r="L47" s="56"/>
-      <c r="M47" s="56"/>
-      <c r="N47" s="56"/>
-      <c r="O47" s="56"/>
-      <c r="P47" s="57"/>
-      <c r="Q47" s="57"/>
-      <c r="R47" s="57"/>
+      <c r="E47" s="57"/>
+      <c r="F47" s="57"/>
+      <c r="G47" s="57"/>
+      <c r="H47" s="57"/>
+      <c r="I47" s="57"/>
+      <c r="J47" s="57"/>
+      <c r="K47" s="57"/>
+      <c r="L47" s="57"/>
+      <c r="M47" s="57"/>
+      <c r="N47" s="57"/>
+      <c r="O47" s="57"/>
+      <c r="P47" s="58"/>
+      <c r="Q47" s="58"/>
+      <c r="R47" s="58"/>
       <c r="U47" s="5"/>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.3">
@@ -2071,101 +2079,101 @@
       <c r="C48" t="s">
         <v>16</v>
       </c>
-      <c r="D48" s="55" t="s">
+      <c r="D48" s="56" t="s">
         <v>59</v>
       </c>
-      <c r="E48" s="56"/>
-      <c r="F48" s="56"/>
-      <c r="G48" s="56"/>
-      <c r="H48" s="56"/>
-      <c r="I48" s="56"/>
-      <c r="J48" s="56"/>
-      <c r="K48" s="56"/>
-      <c r="L48" s="56"/>
-      <c r="M48" s="56"/>
-      <c r="N48" s="56"/>
-      <c r="O48" s="56"/>
-      <c r="P48" s="57"/>
-      <c r="Q48" s="57"/>
-      <c r="R48" s="57"/>
+      <c r="E48" s="57"/>
+      <c r="F48" s="57"/>
+      <c r="G48" s="57"/>
+      <c r="H48" s="57"/>
+      <c r="I48" s="57"/>
+      <c r="J48" s="57"/>
+      <c r="K48" s="57"/>
+      <c r="L48" s="57"/>
+      <c r="M48" s="57"/>
+      <c r="N48" s="57"/>
+      <c r="O48" s="57"/>
+      <c r="P48" s="58"/>
+      <c r="Q48" s="58"/>
+      <c r="R48" s="58"/>
       <c r="U48" s="5"/>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A49" s="4"/>
       <c r="C49" t="s">
         <v>17</v>
       </c>
-      <c r="D49" s="55" t="s">
+      <c r="D49" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="E49" s="56"/>
-      <c r="F49" s="56"/>
-      <c r="G49" s="56"/>
-      <c r="H49" s="56"/>
-      <c r="I49" s="56"/>
-      <c r="J49" s="56"/>
-      <c r="K49" s="56"/>
-      <c r="L49" s="56"/>
-      <c r="M49" s="56"/>
-      <c r="N49" s="56"/>
-      <c r="O49" s="56"/>
-      <c r="P49" s="57"/>
-      <c r="Q49" s="57"/>
-      <c r="R49" s="57"/>
+      <c r="E49" s="57"/>
+      <c r="F49" s="57"/>
+      <c r="G49" s="57"/>
+      <c r="H49" s="57"/>
+      <c r="I49" s="57"/>
+      <c r="J49" s="57"/>
+      <c r="K49" s="57"/>
+      <c r="L49" s="57"/>
+      <c r="M49" s="57"/>
+      <c r="N49" s="57"/>
+      <c r="O49" s="57"/>
+      <c r="P49" s="58"/>
+      <c r="Q49" s="58"/>
+      <c r="R49" s="58"/>
       <c r="U49" s="5"/>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A50" s="4"/>
-      <c r="I50" s="48" t="s">
+      <c r="I50" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="J50" s="48"/>
-      <c r="K50" s="48"/>
-      <c r="L50" s="48"/>
-      <c r="M50" s="48"/>
-      <c r="N50" s="48"/>
-      <c r="O50" s="48"/>
-      <c r="P50" s="48"/>
-      <c r="Q50" s="48"/>
-      <c r="R50" s="48"/>
-      <c r="S50" s="58">
+      <c r="J50" s="49"/>
+      <c r="K50" s="49"/>
+      <c r="L50" s="49"/>
+      <c r="M50" s="49"/>
+      <c r="N50" s="49"/>
+      <c r="O50" s="49"/>
+      <c r="P50" s="49"/>
+      <c r="Q50" s="49"/>
+      <c r="R50" s="49"/>
+      <c r="S50" s="59">
         <f>P45+P46+P47+P48+P49</f>
-        <v>299.35678499999995</v>
-      </c>
-      <c r="T50" s="59"/>
+        <v>327.52178499999997</v>
+      </c>
+      <c r="T50" s="60"/>
       <c r="U50" s="5"/>
     </row>
-    <row r="51" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="4"/>
       <c r="U51" s="5"/>
     </row>
-    <row r="52" spans="1:21" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:24" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="4"/>
       <c r="D52" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="G52" s="60" t="s">
+      <c r="G52" s="61" t="s">
         <v>62</v>
       </c>
-      <c r="H52" s="60"/>
-      <c r="I52" s="60"/>
-      <c r="J52" s="60"/>
-      <c r="K52" s="60"/>
-      <c r="L52" s="60"/>
-      <c r="M52" s="60"/>
-      <c r="N52" s="60"/>
-      <c r="O52" s="60"/>
-      <c r="P52" s="60"/>
-      <c r="Q52" s="60"/>
-      <c r="R52" s="61"/>
-      <c r="S52" s="62">
+      <c r="H52" s="61"/>
+      <c r="I52" s="61"/>
+      <c r="J52" s="61"/>
+      <c r="K52" s="61"/>
+      <c r="L52" s="61"/>
+      <c r="M52" s="61"/>
+      <c r="N52" s="61"/>
+      <c r="O52" s="61"/>
+      <c r="P52" s="61"/>
+      <c r="Q52" s="61"/>
+      <c r="R52" s="62"/>
+      <c r="S52" s="63">
         <f>S36-S50</f>
-        <v>1786.7532149999997</v>
-      </c>
-      <c r="T52" s="63"/>
+        <v>1918.5882149999998</v>
+      </c>
+      <c r="T52" s="64"/>
       <c r="U52" s="5"/>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A53" s="4"/>
       <c r="D53" s="28" t="s">
         <v>64</v>
@@ -2174,43 +2182,52 @@
       <c r="J53" s="19"/>
       <c r="U53" s="5"/>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A54" s="4"/>
-      <c r="G54" s="52"/>
-      <c r="H54" s="52"/>
-      <c r="I54" s="52"/>
+      <c r="G54" s="53" t="s">
+        <v>98</v>
+      </c>
+      <c r="H54" s="53"/>
+      <c r="I54" s="53"/>
       <c r="J54" s="6"/>
-      <c r="K54" s="8"/>
+      <c r="K54" s="8">
+        <v>2025</v>
+      </c>
       <c r="L54" t="s">
         <v>31</v>
       </c>
-      <c r="M54" s="10"/>
-      <c r="N54" s="53"/>
-      <c r="O54" s="53"/>
+      <c r="M54" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="N54" s="54"/>
+      <c r="O54" s="54"/>
       <c r="P54" t="s">
         <v>32</v>
       </c>
+      <c r="Q54">
+        <v>11</v>
+      </c>
       <c r="R54" t="s">
         <v>84</v>
       </c>
       <c r="U54" s="5"/>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A55" s="4"/>
       <c r="U55" s="5"/>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A56" s="4"/>
       <c r="O56" s="29" t="s">
         <v>65</v>
       </c>
       <c r="U56" s="5"/>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A57" s="4"/>
       <c r="U57" s="5"/>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A58" s="9"/>
       <c r="B58" s="10"/>
       <c r="C58" s="10"/>
@@ -2233,7 +2250,7 @@
       <c r="T58" s="10"/>
       <c r="U58" s="12"/>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
       <c r="B61" s="30" t="s">
         <v>66</v>
@@ -2258,31 +2275,31 @@
       <c r="T61" s="31"/>
       <c r="U61" s="3"/>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A62" s="4"/>
       <c r="U62" s="5"/>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A63" s="4"/>
       <c r="C63" t="s">
         <v>11</v>
       </c>
-      <c r="D63" s="45" t="s">
+      <c r="D63" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="E63" s="45"/>
-      <c r="F63" s="45"/>
-      <c r="G63" s="45"/>
-      <c r="H63" s="45"/>
-      <c r="I63" s="45"/>
-      <c r="J63" s="45"/>
-      <c r="K63" s="45"/>
-      <c r="L63" s="45"/>
-      <c r="Q63" s="54" t="s">
+      <c r="E63" s="46"/>
+      <c r="F63" s="46"/>
+      <c r="G63" s="46"/>
+      <c r="H63" s="46"/>
+      <c r="I63" s="46"/>
+      <c r="J63" s="46"/>
+      <c r="K63" s="46"/>
+      <c r="L63" s="46"/>
+      <c r="Q63" s="55" t="s">
         <v>73</v>
       </c>
-      <c r="R63" s="54"/>
-      <c r="S63" s="54" t="s">
+      <c r="R63" s="55"/>
+      <c r="S63" s="55" t="s">
         <v>74</v>
       </c>
       <c r="T63" s="32" t="s">
@@ -2290,49 +2307,52 @@
       </c>
       <c r="U63" s="5"/>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A64" s="4"/>
-      <c r="D64" s="47" t="s">
+      <c r="D64" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="E64" s="47"/>
-      <c r="F64" s="47"/>
-      <c r="G64" s="47"/>
-      <c r="H64" s="47"/>
-      <c r="I64" s="47"/>
-      <c r="J64" s="47"/>
-      <c r="K64" s="47"/>
-      <c r="L64" s="47"/>
-      <c r="M64" s="47"/>
-      <c r="N64" s="47"/>
+      <c r="E64" s="48"/>
+      <c r="F64" s="48"/>
+      <c r="G64" s="48"/>
+      <c r="H64" s="48"/>
+      <c r="I64" s="48"/>
+      <c r="J64" s="48"/>
+      <c r="K64" s="48"/>
+      <c r="L64" s="48"/>
+      <c r="M64" s="48"/>
+      <c r="N64" s="48"/>
       <c r="O64" s="18">
         <f>P13+P15+P16+P17+P22</f>
         <v>2086.1099999999997</v>
       </c>
-      <c r="Q64" s="54"/>
-      <c r="R64" s="54"/>
-      <c r="S64" s="54"/>
+      <c r="Q64" s="55"/>
+      <c r="R64" s="55"/>
+      <c r="S64" s="55"/>
       <c r="T64" s="32" t="s">
         <v>76</v>
       </c>
       <c r="U64" s="5"/>
+      <c r="X64" s="45"/>
     </row>
     <row r="65" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A65" s="4"/>
-      <c r="D65" s="47" t="s">
+      <c r="D65" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="E65" s="47"/>
-      <c r="F65" s="47"/>
-      <c r="G65" s="47"/>
-      <c r="H65" s="47"/>
-      <c r="I65" s="47"/>
-      <c r="J65" s="47"/>
-      <c r="K65" s="47"/>
-      <c r="L65" s="47"/>
-      <c r="M65" s="47"/>
-      <c r="N65" s="47"/>
-      <c r="O65" s="33"/>
+      <c r="E65" s="48"/>
+      <c r="F65" s="48"/>
+      <c r="G65" s="48"/>
+      <c r="H65" s="48"/>
+      <c r="I65" s="48"/>
+      <c r="J65" s="48"/>
+      <c r="K65" s="48"/>
+      <c r="L65" s="48"/>
+      <c r="M65" s="48"/>
+      <c r="N65" s="48"/>
+      <c r="O65" s="33">
+        <v>150</v>
+      </c>
       <c r="Q65" s="23"/>
       <c r="R65" s="23"/>
       <c r="S65" s="23"/>
@@ -2341,32 +2361,32 @@
     </row>
     <row r="66" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A66" s="4"/>
-      <c r="I66" s="48" t="s">
+      <c r="I66" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="J66" s="48"/>
-      <c r="K66" s="48"/>
-      <c r="L66" s="48"/>
-      <c r="M66" s="48"/>
-      <c r="N66" s="48"/>
+      <c r="J66" s="49"/>
+      <c r="K66" s="49"/>
+      <c r="L66" s="49"/>
+      <c r="M66" s="49"/>
+      <c r="N66" s="49"/>
       <c r="O66" s="18">
         <f>+O64+O65</f>
-        <v>2086.1099999999997</v>
+        <v>2236.1099999999997</v>
       </c>
       <c r="P66" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="Q66" s="49">
+      <c r="Q66" s="50">
         <f>+O66</f>
-        <v>2086.1099999999997</v>
-      </c>
-      <c r="R66" s="50"/>
+        <v>2236.1099999999997</v>
+      </c>
+      <c r="R66" s="51"/>
       <c r="S66" s="35">
         <v>23.6</v>
       </c>
       <c r="T66" s="36">
         <f>Q66*0.236</f>
-        <v>492.32195999999988</v>
+        <v>527.72195999999985</v>
       </c>
       <c r="U66" s="5"/>
     </row>
@@ -2390,7 +2410,7 @@
       </c>
       <c r="T67" s="36">
         <f>+Q69*S67/100</f>
-        <v>31.291649999999994</v>
+        <v>35.941649999999996</v>
       </c>
       <c r="U67" s="5"/>
     </row>
@@ -2413,7 +2433,7 @@
       </c>
       <c r="T68" s="36">
         <f>+Q69*S68/100</f>
-        <v>114.73604999999998</v>
+        <v>131.78604999999999</v>
       </c>
       <c r="U68" s="5"/>
     </row>
@@ -2427,22 +2447,22 @@
       </c>
       <c r="O69" s="39">
         <f>P13+P15+P16+P17+P18+P19+P21+P22+(O65)</f>
-        <v>2086.1099999999997</v>
+        <v>2396.1099999999997</v>
       </c>
       <c r="P69" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="Q69" s="49">
+      <c r="Q69" s="50">
         <f>+O69</f>
-        <v>2086.1099999999997</v>
-      </c>
-      <c r="R69" s="50"/>
+        <v>2396.1099999999997</v>
+      </c>
+      <c r="R69" s="51"/>
       <c r="S69" s="35">
         <v>0.6</v>
       </c>
       <c r="T69" s="36">
         <f>+Q69*S69/100</f>
-        <v>12.516659999999996</v>
+        <v>14.376659999999998</v>
       </c>
       <c r="U69" s="5"/>
     </row>
@@ -2452,14 +2472,14 @@
         <v>79</v>
       </c>
       <c r="O70" s="40"/>
-      <c r="Q70" s="51"/>
-      <c r="R70" s="51"/>
+      <c r="Q70" s="52"/>
+      <c r="R70" s="52"/>
       <c r="S70" s="35">
         <v>0.2</v>
       </c>
       <c r="T70" s="36">
         <f>+Q69*S70/100</f>
-        <v>4.1722199999999994</v>
+        <v>4.7922199999999995</v>
       </c>
       <c r="U70" s="5"/>
     </row>
@@ -2468,22 +2488,22 @@
       <c r="C71" t="s">
         <v>20</v>
       </c>
-      <c r="D71" s="45" t="s">
+      <c r="D71" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="E71" s="45"/>
-      <c r="F71" s="45"/>
-      <c r="G71" s="45"/>
-      <c r="H71" s="45"/>
-      <c r="I71" s="45"/>
-      <c r="J71" s="45"/>
-      <c r="K71" s="45"/>
-      <c r="L71" s="45"/>
-      <c r="M71" s="45"/>
-      <c r="N71" s="45"/>
+      <c r="E71" s="46"/>
+      <c r="F71" s="46"/>
+      <c r="G71" s="46"/>
+      <c r="H71" s="46"/>
+      <c r="I71" s="46"/>
+      <c r="J71" s="46"/>
+      <c r="K71" s="46"/>
+      <c r="L71" s="46"/>
+      <c r="M71" s="46"/>
+      <c r="N71" s="46"/>
       <c r="O71" s="18">
         <f>+P18</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="Q71" s="23"/>
       <c r="R71" s="23"/>
@@ -2492,7 +2512,7 @@
       </c>
       <c r="T71" s="36">
         <f>+O71*S71/100</f>
-        <v>0</v>
+        <v>19.2</v>
       </c>
       <c r="U71" s="5"/>
     </row>
@@ -2501,19 +2521,19 @@
       <c r="C72" t="s">
         <v>21</v>
       </c>
-      <c r="D72" s="45" t="s">
+      <c r="D72" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="E72" s="45"/>
-      <c r="F72" s="45"/>
-      <c r="G72" s="45"/>
-      <c r="H72" s="45"/>
-      <c r="I72" s="45"/>
-      <c r="J72" s="45"/>
-      <c r="K72" s="45"/>
-      <c r="L72" s="45"/>
-      <c r="M72" s="45"/>
-      <c r="N72" s="45"/>
+      <c r="E72" s="46"/>
+      <c r="F72" s="46"/>
+      <c r="G72" s="46"/>
+      <c r="H72" s="46"/>
+      <c r="I72" s="46"/>
+      <c r="J72" s="46"/>
+      <c r="K72" s="46"/>
+      <c r="L72" s="46"/>
+      <c r="M72" s="46"/>
+      <c r="N72" s="46"/>
       <c r="O72" s="18">
         <f>+P19</f>
         <v>0</v>
@@ -2534,31 +2554,31 @@
       <c r="C73" t="s">
         <v>22</v>
       </c>
-      <c r="D73" s="45" t="s">
+      <c r="D73" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="E73" s="45"/>
-      <c r="F73" s="45"/>
-      <c r="G73" s="45"/>
-      <c r="H73" s="45"/>
-      <c r="I73" s="45"/>
-      <c r="J73" s="45"/>
-      <c r="K73" s="45"/>
-      <c r="L73" s="45"/>
-      <c r="M73" s="45"/>
-      <c r="N73" s="45"/>
+      <c r="E73" s="46"/>
+      <c r="F73" s="46"/>
+      <c r="G73" s="46"/>
+      <c r="H73" s="46"/>
+      <c r="I73" s="46"/>
+      <c r="J73" s="46"/>
+      <c r="K73" s="46"/>
+      <c r="L73" s="46"/>
+      <c r="M73" s="46"/>
+      <c r="N73" s="46"/>
       <c r="O73" s="18">
         <f>S36</f>
-        <v>2086.1099999999997</v>
+        <v>2246.1099999999997</v>
       </c>
       <c r="Q73" s="23"/>
-      <c r="R73" s="46" t="s">
+      <c r="R73" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="S73" s="46"/>
+      <c r="S73" s="47"/>
       <c r="T73" s="41">
         <f>+T66+T67+T68+T69+T70+T71+T72</f>
-        <v>655.0385399999999</v>
+        <v>733.81853999999987</v>
       </c>
       <c r="U73" s="5"/>
     </row>
@@ -2684,6 +2704,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100FAD20F2317B007458AE410145ECF2664" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="faedee2b1d17e4a9aacad85634c645fb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="15953625-9918-4c64-bfaa-da99dd23a1f9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3ec38d02a41af380e46befe1a010f701" ns2:_="">
     <xsd:import namespace="15953625-9918-4c64-bfaa-da99dd23a1f9"/>
@@ -2827,22 +2862,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51A13B28-BE0D-4F84-8A7A-45272EF286DD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B95B890-0ABD-4B96-AA6E-1E41EF93328F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="15953625-9918-4c64-bfaa-da99dd23a1f9"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49142F88-2D5A-4E31-A291-FE22E6D45562}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2858,28 +2902,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51A13B28-BE0D-4F84-8A7A-45272EF286DD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B95B890-0ABD-4B96-AA6E-1E41EF93328F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="15953625-9918-4c64-bfaa-da99dd23a1f9"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>